<commit_message>
Code updated 23-01-19 11:32:03
</commit_message>
<xml_diff>
--- a/Season_Trophies/82.xlsx
+++ b/Season_Trophies/82.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,17 +396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>29214</t>
+          <t>45275</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>春田花花幼稚园</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2781</t>
+          <t>2632</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26424998</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
+          <t>摸鱼者三战</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3785</t>
+          <t>3530</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2382</t>
+          <t>43321</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3421</t>
+          <t>2662</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2949</t>
+          <t>50050</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21345373</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>林北不講武德</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3395</t>
+          <t>2564</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7884</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>摸鱼者三战</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,186 +524,186 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3209</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>13582</t>
+          <t>24223</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32478707</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"Bt So"</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3056</t>
+          <t>3005</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>26624</t>
+          <t>19779</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2820</t>
+          <t>3107</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>37709</t>
+          <t>5602</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2662</t>
+          <t>3565</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>45617</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2564</t>
+          <t>3563</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>46991</t>
+          <t>8450</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2550</t>
+          <t>3446</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>8478</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>43812707</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>bbtt</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3445</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19610</t>
+          <t>14504</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2938</t>
+          <t>3245</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>26922</t>
+          <t>15253</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2815</t>
+          <t>3223</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3588</t>
+          <t>19926</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3364</t>
+          <t>3104</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>7673</t>
+          <t>19949</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3215</t>
+          <t>3103</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>8488</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>45070827</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>㊥山东老灶丿</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3188</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>10982</t>
+          <t>4096</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>Kikkik</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3117</t>
+          <t>3640</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>13557</t>
+          <t>5188</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3056</t>
+          <t>3584</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18078</t>
+          <t>5571</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2968</t>
+          <t>3566</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>22779</t>
+          <t>7214</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2882</t>
+          <t>3495</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>24675</t>
+          <t>10068</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2850</t>
+          <t>3386</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>9635</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>45070827</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>㊥山东老灶丿</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3400</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2716</t>
+          <t>11318</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Kikkik</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3405</t>
+          <t>3342</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4151</t>
+          <t>12244</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>47758619</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"㊥ Moon ㊥"</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3340</t>
+          <t>3312</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6724</t>
+          <t>14731</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>3248</t>
+          <t>3238</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6817</t>
+          <t>17925</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>12639656</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>"wu huang"</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>3245</t>
+          <t>3154</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6966</t>
+          <t>18340</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3240</t>
+          <t>3143</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>9459</t>
+          <t>18346</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>54915122</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>平胸救世界</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3160</t>
+          <t>3143</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>11101</t>
+          <t>18490</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3114</t>
+          <t>3140</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12015</t>
+          <t>20162</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>3092</t>
+          <t>3098</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12615</t>
+          <t>20418</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>3079</t>
+          <t>3093</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>15274</t>
+          <t>26462</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3018</t>
+          <t>2962</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>16691</t>
+          <t>27521</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>2941</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>16907</t>
+          <t>33483</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2989</t>
+          <t>2826</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>18742</t>
+          <t>33900</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2955</t>
+          <t>2818</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19445</t>
+          <t>34786</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2942</t>
+          <t>2803</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19958</t>
+          <t>35141</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2931</t>
+          <t>2797</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>22621</t>
+          <t>39981</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>54915122</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>平胸救世界</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2884</t>
+          <t>2714</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>24884</t>
+          <t>40410</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2847</t>
+          <t>2708</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>27023</t>
+          <t>44068</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2813</t>
+          <t>2650</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>28561</t>
+          <t>45986</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2790</t>
+          <t>2621</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>31904</t>
+          <t>46055</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2742</t>
+          <t>2620</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>33054</t>
+          <t>51872</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>25435189</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2726</t>
+          <t>2544</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>35394</t>
+          <t>58231</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2693</t>
+          <t>2488</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>37030</t>
+          <t>82013</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>57837683</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>我的世界只有你</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,240 +1604,240 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2671</t>
+          <t>2003</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>40766</t>
+          <t>13060</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2621</t>
+          <t>3287</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>40809</t>
+          <t>2631</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2621</t>
+          <t>3724</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>44070</t>
+          <t>4436</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2581</t>
+          <t>3621</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>50324</t>
+          <t>5260</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>25435189</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2519</t>
+          <t>3581</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>53157</t>
+          <t>7116</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>3499</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>53518</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2499</t>
+          <t>3499</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>77682</t>
+          <t>7582</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>57837683</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>我的世界只有你</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>3481</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>8069</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>5691528</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>ABearBear</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3460</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>16638</t>
+          <t>10125</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2993</t>
+          <t>3384</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6948</t>
+          <t>16194</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,14 +1874,14 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3241</t>
+          <t>3198</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>25441</t>
+          <t>25976</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1901,14 +1901,14 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2838</t>
+          <t>2972</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>45718</t>
+          <t>48027</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2563</t>
+          <t>2591</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2276</t>
+          <t>15079</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>3427</t>
+          <t>3228</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3884</t>
+          <t>17269</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3351</t>
+          <t>3170</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>3981</t>
+          <t>20423</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>51841127</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t>"Muhammad Shox"</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3347</t>
+          <t>3093</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>4670</t>
+          <t>21038</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7857221</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Rename</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3321</t>
+          <t>3080</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7818</t>
+          <t>22658</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3210</t>
+          <t>3042</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>8798</t>
+          <t>25112</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6940556</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>3179</t>
+          <t>2988</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>10413</t>
+          <t>29000</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>3132</t>
+          <t>2910</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>12696</t>
+          <t>29064</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5691528</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ABearBear</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>3076</t>
+          <t>2909</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>12969</t>
+          <t>30561</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>3070</t>
+          <t>2881</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>13983</t>
+          <t>30236</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>3047</t>
+          <t>2886</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>16540</t>
+          <t>31300</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2995</t>
+          <t>2867</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>19715</t>
+          <t>33513</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2936</t>
+          <t>2825</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20932</t>
+          <t>33814</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>51841127</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"Muhammad Shox"</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2913</t>
+          <t>2820</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>23102</t>
+          <t>34888</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2876</t>
+          <t>2801</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>23544</t>
+          <t>35806</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2869</t>
+          <t>2786</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>23820</t>
+          <t>36987</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2865</t>
+          <t>2766</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>27973</t>
+          <t>38372</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2798</t>
+          <t>2742</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>29253</t>
+          <t>41513</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2780</t>
+          <t>2690</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>30283</t>
+          <t>48077</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>9321819</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>"Mohit Rojasara"</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2766</t>
+          <t>2590</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>33366</t>
+          <t>48689</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2721</t>
+          <t>2582</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>36479</t>
+          <t>49058</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2678</t>
+          <t>2578</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>35817</t>
+          <t>49166</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2687</t>
+          <t>2576</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>40479</t>
+          <t>49668</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2625</t>
+          <t>2570</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>44867</t>
+          <t>51167</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2573</t>
+          <t>2552</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>43864</t>
+          <t>52912</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>AdyYouTubeSs</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2583</t>
+          <t>2531</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>44590</t>
+          <t>54453</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2576</t>
+          <t>2516</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>47153</t>
+          <t>55304</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2548</t>
+          <t>2508</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>49255</t>
+          <t>59454</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>47227626</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>Player-47227626</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>2478</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>49621</t>
+          <t>62302</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2525</t>
+          <t>2452</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>49693</t>
+          <t>62443</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2524</t>
+          <t>2451</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>48719</t>
+          <t>63383</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,24 +2765,24 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2533</t>
+          <t>2440</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>52730</t>
+          <t>67509</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2792,24 +2792,24 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2501</t>
+          <t>2369</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>55641</t>
+          <t>68590</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2487</t>
+          <t>2308</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>58194</t>
+          <t>71830</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,240 +2846,240 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2472</t>
+          <t>2170</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>59761</t>
+          <t>36691</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2460</t>
+          <t>2771</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>60064</t>
+          <t>2860</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>AdyYouTubeSs</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2458</t>
+          <t>3709</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>63340</t>
+          <t>9893</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2431</t>
+          <t>3392</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>64225</t>
+          <t>37543</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2420</t>
+          <t>2757</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>65690</t>
+          <t>51755</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2395</t>
+          <t>2545</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>66579</t>
+          <t>727</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2356</t>
+          <t>3918</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>66612</t>
+          <t>864</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>"Zephyr ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2353</t>
+          <t>3893</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>69317</t>
+          <t>1057</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2173</t>
+          <t>3867</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>43812</t>
+          <t>1591</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>㊥JOSE</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2584</t>
+          <t>3806</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>3271</t>
+          <t>1815</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>11783968</t>
+          <t>20199374</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>F---119</t>
+          <t>RuanFan</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3379</t>
+          <t>3784</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>9459</t>
+          <t>2027</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3160</t>
+          <t>3767</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>36336</t>
+          <t>2337</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2680</t>
+          <t>3744</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>55847</t>
+          <t>2677</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2486</t>
+          <t>3721</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>1418</t>
+          <t>3028</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>㊥JOSE</t>
+          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>3484</t>
+          <t>3699</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>622</t>
+          <t>3747</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>"Zephyr ᶻᵍˣ"</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>3567</t>
+          <t>3657</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>3919</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>20199374</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>RuanFan</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3445</t>
+          <t>3648</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2408</t>
+          <t>4898</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>21345373</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>林北不講武德</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3420</t>
+          <t>3598</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2865</t>
+          <t>5634</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3398</t>
+          <t>3564</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>3197</t>
+          <t>5765</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>3382</t>
+          <t>3558</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>3235</t>
+          <t>7937</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>3380</t>
+          <t>3465</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>3619</t>
+          <t>8465</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>3362</t>
+          <t>3446</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>3718</t>
+          <t>9243</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>32613475</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>"李 无 善 德"</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>3358</t>
+          <t>3415</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>6464</t>
+          <t>10670</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3258</t>
+          <t>3365</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>7065</t>
+          <t>11084</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>32478707</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>"Bt So"</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>3236</t>
+          <t>3351</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>8062</t>
+          <t>12429</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>3202</t>
+          <t>3306</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>10683</t>
+          <t>12487</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>3124</t>
+          <t>3304</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>10812</t>
+          <t>13319</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>3121</t>
+          <t>3280</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>12355</t>
+          <t>16392</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>3085</t>
+          <t>3193</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>13304</t>
+          <t>18059</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>3062</t>
+          <t>3150</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>13750</t>
+          <t>18106</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>3052</t>
+          <t>3149</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>17853</t>
+          <t>19517</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2972</t>
+          <t>3113</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>20586</t>
+          <t>19845</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2920</t>
+          <t>3106</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>25839</t>
+          <t>21788</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>春田花花幼稚园</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2832</t>
+          <t>3063</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>28411</t>
+          <t>30379</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,24 +3764,24 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2792</t>
+          <t>2884</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>28507</t>
+          <t>43146</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3791,24 +3791,24 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2791</t>
+          <t>2665</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>42747</t>
+          <t>43495</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>54924790</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>Sujit4u</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,24 +3818,24 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2596</t>
+          <t>2659</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>52956</t>
+          <t>53758</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3845,24 +3845,24 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2522</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>79532</t>
+          <t>54030</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>57722377</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>VI空白IV</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>2519</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>81059</t>
+          <t>81722</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>57867293</t>
+          <t>57722377</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Player-57867293</t>
+          <t>VI空白IV</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>2006</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>100643</t>
+          <t>84815</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>57867293</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Player-57867293</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,78 +3926,78 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>1498</t>
+          <t>1987</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>90309</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1728</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>14216</t>
+          <t>94070</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>3041</t>
+          <t>1593</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>36219</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2682</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>52935</t>
+          <t>13794</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>3265</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>57798</t>
+          <t>21881</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,24 +4061,24 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2475</t>
+          <t>3061</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>37525</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2757</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>45358</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,7 +4115,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -4127,12 +4127,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4154,20 +4154,74 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
+          <t>9195340</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Namllllllik</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>8850180</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>30624300</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
           <t>28624723</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr">
+      <c r="C143" t="inlineStr">
         <is>
           <t>"Woody Shade"</t>
         </is>
       </c>
-      <c r="D141" t="inlineStr">
+      <c r="D143" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E141" t="inlineStr">
+      <c r="E143" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-01-29 11:30:33
</commit_message>
<xml_diff>
--- a/Season_Trophies/82.xlsx
+++ b/Season_Trophies/82.xlsx
@@ -396,17 +396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>57792</t>
+          <t>23362</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>春田花花幼稚园</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2772</t>
+          <t>4416</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>259</t>
+          <t>5992</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26424998</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>7109</t>
+          <t>6054</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>3517</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>摸鱼者三战</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7055</t>
+          <t>6411</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>487</t>
+          <t>3403</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>20199374</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>RuanFan</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7004</t>
+          <t>6434</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>568</t>
+          <t>4149</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6966</t>
+          <t>6299</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>626</t>
+          <t>3080</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>㊥JOSE</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6937</t>
+          <t>6498</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>7642</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6940556</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6914</t>
+          <t>5750</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>718</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32613475</t>
+          <t>5691528</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"李 无 善 德"</t>
+          <t>ABearBear</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6904</t>
+          <t>6188</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1436</t>
+          <t>8404</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6668</t>
+          <t>5621</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1828</t>
+          <t>624</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>7216</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2609</t>
+          <t>3641</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6367</t>
+          <t>6389</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2826</t>
+          <t>51272</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11783968</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>F---119</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6324</t>
+          <t>3047</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2788</t>
+          <t>601</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6331</t>
+          <t>7227</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2945</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6048</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3256</t>
+          <t>2478</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6237</t>
+          <t>6625</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3340</t>
+          <t>29103</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>摸鱼者三战</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>6221</t>
+          <t>4056</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3944</t>
+          <t>8954</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6114</t>
+          <t>5543</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4188</t>
+          <t>4273</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6081</t>
+          <t>6279</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4352</t>
+          <t>382</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>20199374</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>RuanFan</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6058</t>
+          <t>7329</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4392</t>
+          <t>6470</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6052</t>
+          <t>6002</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4403</t>
+          <t>5470</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>21345373</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>林北不講武德</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6051</t>
+          <t>6114</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4530</t>
+          <t>8106</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6033</t>
+          <t>5670</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4545</t>
+          <t>2647</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>27113069</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>㊥DumbSmoky</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6031</t>
+          <t>6588</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6013</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4855</t>
+          <t>6723</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>Kikkik</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5991</t>
+          <t>5947</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4919</t>
+          <t>1911</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>21345373</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>林北不講武德</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5982</t>
+          <t>6784</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5023</t>
+          <t>3407</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5691528</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ABearBear</t>
+          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5965</t>
+          <t>6433</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5407</t>
+          <t>286</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5911</t>
+          <t>7374</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5890</t>
+          <t>4039</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5849</t>
+          <t>6317</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>3241</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>32478707</t>
+          <t>27113069</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>"Bt So"</t>
+          <t>㊥DumbSmoky</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5817</t>
+          <t>6466</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6440</t>
+          <t>2280</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5769</t>
+          <t>6679</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>2352</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t>Auto-Battle</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5758</t>
+          <t>6658</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>7005</t>
+          <t>53937</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Kikkik</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>2935</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>7239</t>
+          <t>1859</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>5641</t>
+          <t>6798</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>7638</t>
+          <t>5920</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>6063</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>7761</t>
+          <t>11432</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>5555</t>
+          <t>5301</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>8255</t>
+          <t>4718</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>5486</t>
+          <t>6215</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>10016</t>
+          <t>6874</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>5280</t>
+          <t>5910</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>14085</t>
+          <t>408</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4918</t>
+          <t>7316</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>48897</t>
+          <t>5552</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>32478707</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>"Bt So"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3112</t>
+          <t>6103</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>50278</t>
+          <t>731</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3047</t>
+          <t>7170</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>52975</t>
+          <t>3758</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2935</t>
+          <t>6366</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>5010</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,186 +1550,186 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6169</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>17234</t>
+          <t>8146</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4675</t>
+          <t>5664</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>18514</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4596</t>
+          <t>6343</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3597</t>
+          <t>49955</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>6170</t>
+          <t>3112</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7961</t>
+          <t>3009</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5529</t>
+          <t>6514</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>8680</t>
+          <t>14449</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5429</t>
+          <t>5015</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>12076</t>
+          <t>900</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>㊥JOSE</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>5102</t>
+          <t>7116</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>14837</t>
+          <t>64705</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4853</t>
+          <t>2608</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>17652</t>
+          <t>39470</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4646</t>
+          <t>3564</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>32174</t>
+          <t>50850</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3839</t>
+          <t>3067</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>6573</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>45070827</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>㊥山东老灶丿</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5983</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6389</t>
+          <t>19977</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>5779</t>
+          <t>4614</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7144</t>
+          <t>18356</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>4699</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>8479</t>
+          <t>7267</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>5453</t>
+          <t>5823</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>10286</t>
+          <t>16334</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,14 +1928,14 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>5257</t>
+          <t>4843</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>10807</t>
+          <t>11007</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5213</t>
+          <t>5336</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>11224</t>
+          <t>48273</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>12639656</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>"wu huang"</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5175</t>
+          <t>3195</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>13440</t>
+          <t>10467</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4978</t>
+          <t>5381</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>14219</t>
+          <t>35172</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>4907</t>
+          <t>3781</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>15687</t>
+          <t>45620</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>4779</t>
+          <t>3304</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>16959</t>
+          <t>10162</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>4692</t>
+          <t>5409</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>17871</t>
+          <t>54051</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>25435189</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>4633</t>
+          <t>2930</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>18797</t>
+          <t>4241</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>47758619</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>"㊥ Moon ㊥"</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>4581</t>
+          <t>6284</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20859</t>
+          <t>17686</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>4468</t>
+          <t>4744</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>21378</t>
+          <t>18791</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>4436</t>
+          <t>4676</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>22003</t>
+          <t>16569</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>54915122</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>平胸救世界</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4400</t>
+          <t>4824</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>22618</t>
+          <t>23252</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4363</t>
+          <t>4425</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>23926</t>
+          <t>19648</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4274</t>
+          <t>4630</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>26260</t>
+          <t>20530</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4128</t>
+          <t>4589</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>32129</t>
+          <t>26924</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3841</t>
+          <t>4173</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>33810</t>
+          <t>10561</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>5373</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>37838</t>
+          <t>7856</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>43812707</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>bbtt</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>3580</t>
+          <t>5715</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>39855</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>45070827</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>㊥山东老灶丿</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>3488</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>44041</t>
+          <t>9226</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>3318</t>
+          <t>5508</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>47088</t>
+          <t>20710</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>3195</t>
+          <t>4581</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>47458</t>
+          <t>13950</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3178</t>
+          <t>5063</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>48222</t>
+          <t>11717</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>56829330</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>"FLO ALX"</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3142</t>
+          <t>5279</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>50561</t>
+          <t>12778</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>3036</t>
+          <t>5198</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>52514</t>
+          <t>16797</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2954</t>
+          <t>4807</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>54755</t>
+          <t>21787</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>25435189</t>
+          <t>54915122</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>平胸救世界</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2869</t>
+          <t>4528</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>63932</t>
+          <t>31779</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2608</t>
+          <t>3931</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>91205</t>
+          <t>30986</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>57837683</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>我的世界只有你</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,213 +2657,213 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2087</t>
+          <t>3968</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>13730</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>5805</t>
+          <t>5085</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>27387</t>
+          <t>48983</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>4064</t>
+          <t>3160</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>49294</t>
+          <t>38082</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>3093</t>
+          <t>3631</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>9964</t>
+          <t>44912</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>56829330</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>"FLO ALX"</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>5285</t>
+          <t>3332</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>17238</t>
+          <t>55456</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>4675</t>
+          <t>2878</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>18402</t>
+          <t>91379</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>57837683</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>我的世界只有你</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>4603</t>
+          <t>2102</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>20357</t>
+          <t>51485</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>51841127</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>"Muhammad Shox"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>4498</t>
+          <t>3037</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>23453</t>
+          <t>53074</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>4305</t>
+          <t>2969</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>23744</t>
+          <t>48309</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>4287</t>
+          <t>3193</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>25421</t>
+          <t>76660</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>4180</t>
+          <t>2386</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>27193</t>
+          <t>75377</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>4074</t>
+          <t>2417</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>27516</t>
+          <t>25271</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>4058</t>
+          <t>4278</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>28556</t>
+          <t>91819</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4003</t>
+          <t>2094</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>29393</t>
+          <t>28131</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3964</t>
+          <t>4103</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>29523</t>
+          <t>65728</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>Player-20372140</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>3958</t>
+          <t>2587</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>29526</t>
+          <t>18890</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>3957</t>
+          <t>4671</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>32488</t>
+          <t>25845</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3826</t>
+          <t>4238</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>32705</t>
+          <t>23338</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3816</t>
+          <t>4418</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>35309</t>
+          <t>19379</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>3695</t>
+          <t>4645</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>36606</t>
+          <t>22550</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3637</t>
+          <t>4487</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>41336</t>
+          <t>59199</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>3426</t>
+          <t>2754</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>42078</t>
+          <t>56532</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>3395</t>
+          <t>2839</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>42405</t>
+          <t>5872</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3381</t>
+          <t>6067</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>44989</t>
+          <t>27399</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3279</t>
+          <t>4147</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>46534</t>
+          <t>30056</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3219</t>
+          <t>4010</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>48569</t>
+          <t>56970</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>47227626</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>Player-47227626</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>3126</t>
+          <t>2824</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>49785</t>
+          <t>38068</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>3070</t>
+          <t>3632</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>52248</t>
+          <t>35732</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2966</t>
+          <t>3749</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>56674</t>
+          <t>33087</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2804</t>
+          <t>3877</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>62751</t>
+          <t>19932</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>51841127</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>"Muhammad Shox"</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2634</t>
+          <t>4616</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>62944</t>
+          <t>62483</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>58615957</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Anesu597386</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2629</t>
+          <t>2662</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>64594</t>
+          <t>48105</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Player-20372140</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2595</t>
+          <t>3202</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>70672</t>
+          <t>32926</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2492</t>
+          <t>3884</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>73492</t>
+          <t>48371</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>2442</t>
+          <t>3190</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>74337</t>
+          <t>27767</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2424</t>
+          <t>4123</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>75406</t>
+          <t>40165</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2399</t>
+          <t>3533</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>90712</t>
+          <t>29492</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>2096</t>
+          <t>4037</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>104565</t>
+          <t>49198</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,213 +3683,213 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>1770</t>
+          <t>3148</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>58369</t>
+          <t>43135</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2754</t>
+          <t>3404</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>9157</t>
+          <t>41562</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>5368</t>
+          <t>3470</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>29533</t>
+          <t>31337</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>3957</t>
+          <t>3951</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>71964</t>
+          <t>44362</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2471</t>
+          <t>3354</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>91732</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Auto-Battle</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>6613</t>
+          <t>2095</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>1917</t>
+          <t>73180</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>6533</t>
+          <t>2463</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>6160</t>
+          <t>51529</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>5814</t>
+          <t>3035</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>25821</t>
+          <t>59547</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>春田花花幼稚园</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>4155</t>
+          <t>2744</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>37542</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>46248210</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>Ajay</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>3593</t>
+          <t>1062</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>40868</t>
+          <t>75401</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>47533851</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>Bibek</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>3445</t>
+          <t>2417</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>50169</t>
+          <t>30658</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>54924790</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Sujit4u</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>3052</t>
+          <t>3982</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>52169</t>
+          <t>42196</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2968</t>
+          <t>3445</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>54133</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>50742014</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>"Aditya Naik"</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2892</t>
+          <t>996</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>54266</t>
+          <t>94252</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>54714516</t>
+          <t>53269862</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>ёмιいч</t>
+          <t>New_Player111</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,24 +4061,24 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2887</t>
+          <t>2051</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>54713</t>
+          <t>48939</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>54714516</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>ёмιいч</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>2870</t>
+          <t>3162</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>76134</t>
+          <t>49597</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>55963040</t>
+          <t>54924790</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Baliram</t>
+          <t>Sujit4u</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2382</t>
+          <t>3128</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>76805</t>
+          <t>54775</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>2366</t>
+          <t>2902</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>77781</t>
+          <t>77232</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>47533851</t>
+          <t>55963040</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Bibek</t>
+          <t>Baliram</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>2344</t>
+          <t>2373</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>88125</t>
+          <t>72072</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>57722377</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>VI空白IV</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,24 +4196,24 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>2152</t>
+          <t>2482</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>92977</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>53269862</t>
+          <t>56691087</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>New_Player111</t>
+          <t>LongestSovereign8</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,24 +4223,24 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>2057</t>
+          <t>1883</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>95667</t>
+          <t>55063</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>57867293</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Player-57867293</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4250,24 +4250,24 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2892</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>101088</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>56691087</t>
+          <t>57339836</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>LongestSovereign8</t>
+          <t>Player-57339836</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,24 +4277,24 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1883</t>
+          <t>1167</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>107308</t>
+          <t>88512</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>58644547</t>
+          <t>57722377</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>RotaryPreparation39</t>
+          <t>VI空白IV</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4304,24 +4304,24 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>1712</t>
+          <t>2164</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>112203</t>
+          <t>95527</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58635041</t>
+          <t>57867293</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Player-58635041</t>
+          <t>Player-57867293</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,24 +4331,24 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1635</t>
+          <t>2030</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>118207</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>57605565</t>
+          <t>58132159</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>"Leonel Messi"</t>
+          <t>ExultantDelivery42</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,24 +4358,24 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1559</t>
+          <t>1514</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>122899</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>58132159</t>
+          <t>58562596</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>ExultantDelivery42</t>
+          <t>Player-58562596</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,24 +4385,24 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1514</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>133621</t>
+          <t>74070</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>58689512</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Player-58689512</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,24 +4412,24 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>1441</t>
+          <t>2445</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>157006</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>58705573</t>
+          <t>58635041</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Player-58705573</t>
+          <t>Player-58635041</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4439,24 +4439,24 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>1274</t>
+          <t>1587</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>174001</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>57339836</t>
+          <t>58644547</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Player-57339836</t>
+          <t>RotaryPreparation39</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4466,24 +4466,24 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>1167</t>
+          <t>1733</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>228192</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>58562596</t>
+          <t>58689512</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Player-58562596</t>
+          <t>Player-58689512</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4493,24 +4493,24 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1637</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>300945</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>50742014</t>
+          <t>58705573</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>"Aditya Naik"</t>
+          <t>Player-58705573</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4520,24 +4520,24 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>997</t>
+          <t>1304</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>47462</t>
+          <t>7268</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4547,24 +4547,24 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>3178</t>
+          <t>5823</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>4603</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4574,24 +4574,24 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>6022</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>6816</t>
+          <t>67538</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4601,24 +4601,24 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>5714</t>
+          <t>2550</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>42881</t>
+          <t>4247</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4628,24 +4628,24 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>3364</t>
+          <t>6282</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>66793</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4655,24 +4655,24 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>2550</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>42551</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -4682,24 +4682,24 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3430</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>28624723</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"Woody Shade"</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -4716,17 +4716,17 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>48027</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -4736,14 +4736,14 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3206</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>61656</t>
+          <t>63473</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>2661</t>
+          <t>2636</t>
         </is>
       </c>
     </row>

</xml_diff>